<commit_message>
Multibody Dynamics Systems Theory Final Commit
</commit_message>
<xml_diff>
--- a/mbs Stabilization Debug/mbs-EP-Baumgarte/Excel Files/template_mbs.xlsx
+++ b/mbs Stabilization Debug/mbs-EP-Baumgarte/Excel Files/template_mbs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs-EP-v.1.0.0\Excel Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago_Serralha\Desktop\Thesis-Project\mbs Stabilization Debug\mbs-EP-Baumgarte\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE8E3C-2655-4E0A-8312-ADAEC3C49FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4847FE-D5CD-476F-9575-C777E3BDD879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="510" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimParam" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="142">
   <si>
     <t>Mass</t>
   </si>
@@ -841,6 +841,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,13 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -868,7 +871,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -880,15 +889,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -904,18 +904,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,30 +947,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE954C49-6E73-4D49-8054-42AF7A10140C}">
   <dimension ref="B2:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C3" s="55"/>
       <c r="D3" s="30">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>22</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="30">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>22</v>
@@ -1445,9 +1445,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="49"/>
-      <c r="D6" s="30" t="s">
-        <v>3</v>
-      </c>
+      <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
         <v>88</v>
       </c>
@@ -1470,9 +1468,7 @@
         <v>89</v>
       </c>
       <c r="C7" s="49"/>
-      <c r="D7" s="30">
-        <v>-9806.65</v>
-      </c>
+      <c r="D7" s="30"/>
       <c r="E7" s="32" t="s">
         <v>118</v>
       </c>
@@ -1558,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -1578,8 +1574,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="56"/>
-      <c r="B1" s="56"/>
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="50" t="s">
         <v>30</v>
       </c>
@@ -1627,23 +1623,23 @@
       <c r="AK1" s="50"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="58" t="s">
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58" t="s">
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
       <c r="L2" s="50" t="s">
         <v>33</v>
       </c>
@@ -1654,27 +1650,27 @@
       </c>
       <c r="P2" s="50"/>
       <c r="Q2" s="50"/>
-      <c r="R2" s="59" t="s">
+      <c r="R2" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="57" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="58" t="s">
+      <c r="S2" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
       <c r="W2" s="50" t="s">
         <v>101</v>
       </c>
       <c r="X2" s="50"/>
       <c r="Y2" s="50"/>
-      <c r="Z2" s="60" t="s">
+      <c r="Z2" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="57"/>
+      <c r="AB2" s="58"/>
       <c r="AC2" s="50" t="s">
         <v>99</v>
       </c>
@@ -1743,8 +1739,8 @@
       <c r="Q3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="57"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="60"/>
       <c r="T3" s="17" t="s">
         <v>69</v>
       </c>
@@ -5328,12 +5324,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="S1:AK1"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:V2"/>
@@ -5347,6 +5337,12 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="C1:E1"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="S1:AK1"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5378,16 +5374,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -5418,11 +5414,11 @@
       <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -5494,19 +5490,19 @@
       <c r="X4" s="10"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
@@ -5531,16 +5527,16 @@
       <c r="E6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="67"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="66" t="s">
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="68"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
@@ -5576,22 +5572,22 @@
       <c r="X7" s="10"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -5616,21 +5612,21 @@
       <c r="E9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="65" t="s">
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65" t="s">
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -5712,19 +5708,19 @@
       <c r="X11" s="10"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
@@ -5749,16 +5745,16 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65" t="s">
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -5836,19 +5832,19 @@
       <c r="X16" s="10"/>
     </row>
     <row r="17" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="63"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
@@ -5873,16 +5869,16 @@
       <c r="E18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="65" t="s">
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
     </row>
     <row r="19" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
@@ -5919,19 +5915,19 @@
       <c r="X20" s="10"/>
     </row>
     <row r="21" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
@@ -5956,16 +5952,16 @@
       <c r="E22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="65" t="s">
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
     </row>
     <row r="23" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
@@ -6004,22 +6000,22 @@
     </row>
     <row r="24" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
-      <c r="L25" s="63"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
     </row>
     <row r="26" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
@@ -6037,44 +6033,44 @@
       <c r="E26" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="64" t="s">
+      <c r="F26" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="65" t="s">
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65" t="s">
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
     </row>
     <row r="27" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:24" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
     </row>
     <row r="30" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
@@ -6092,26 +6088,26 @@
       <c r="E30" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="66" t="s">
+      <c r="F30" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="67"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="66" t="s">
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="65" t="s">
+      <c r="J30" s="70"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="M30" s="65"/>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65" t="s">
+      <c r="M30" s="63"/>
+      <c r="N30" s="63"/>
+      <c r="O30" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="63"/>
     </row>
     <row r="31" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
@@ -6134,14 +6130,14 @@
     </row>
     <row r="32" spans="1:24" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -6215,12 +6211,12 @@
       <c r="X36" s="10"/>
     </row>
     <row r="37" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -6292,15 +6288,15 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="69" t="s">
+      <c r="A41" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="71"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="68"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
       <c r="J41" s="10"/>
@@ -6320,11 +6316,11 @@
       <c r="D42" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="65" t="s">
+      <c r="E42" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="10"/>
@@ -6448,6 +6444,21 @@
     <row r="64" spans="1:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="A17:K17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="A21:K21"/>
     <mergeCell ref="F22:H22"/>
@@ -6464,21 +6475,6 @@
     <mergeCell ref="I30:K30"/>
     <mergeCell ref="L30:N30"/>
     <mergeCell ref="O30:Q30"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="A17:K17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -6595,7 +6591,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:P13"/>
+      <selection activeCell="B10" sqref="B10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6617,56 +6613,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="81" t="s">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="83"/>
-      <c r="U2" s="84" t="s">
+      <c r="N2" s="90"/>
+      <c r="O2" s="90"/>
+      <c r="P2" s="90"/>
+      <c r="Q2" s="90"/>
+      <c r="R2" s="91"/>
+      <c r="U2" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
     </row>
     <row r="3" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
@@ -6684,16 +6680,16 @@
       <c r="E3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="77" t="s">
+      <c r="G3" s="79"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
       <c r="L3" s="44" t="s">
         <v>123</v>
       </c>
@@ -6709,133 +6705,113 @@
       <c r="P3" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="Q3" s="88" t="s">
+      <c r="Q3" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="R3" s="88"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
+      <c r="R3" s="82"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
+      <c r="Z3" s="77"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="48" t="s">
-        <v>79</v>
-      </c>
+      <c r="B4" s="48"/>
       <c r="C4" s="48"/>
-      <c r="D4" s="48">
-        <v>2</v>
-      </c>
-      <c r="E4" s="48">
-        <v>4</v>
-      </c>
-      <c r="F4" s="48">
-        <v>0</v>
-      </c>
-      <c r="G4" s="48">
-        <v>0</v>
-      </c>
-      <c r="H4" s="48">
-        <v>0</v>
-      </c>
-      <c r="I4" s="48">
-        <v>663</v>
-      </c>
-      <c r="J4" s="48">
-        <v>0</v>
-      </c>
-      <c r="K4" s="48">
-        <v>0</v>
-      </c>
-      <c r="L4" s="19">
-        <v>1</v>
-      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="19"/>
       <c r="M4" s="45"/>
       <c r="N4" s="19"/>
       <c r="O4" s="19"/>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="84"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
+      <c r="Z4" s="77"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="L5" s="19"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="84"/>
-      <c r="Z5" s="84"/>
+      <c r="U5" s="77"/>
+      <c r="V5" s="77"/>
+      <c r="W5" s="77"/>
+      <c r="X5" s="77"/>
+      <c r="Y5" s="77"/>
+      <c r="Z5" s="77"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U6" s="84"/>
-      <c r="V6" s="84"/>
-      <c r="W6" s="84"/>
-      <c r="X6" s="84"/>
-      <c r="Y6" s="84"/>
-      <c r="Z6" s="84"/>
+      <c r="U6" s="77"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="77"/>
+      <c r="X6" s="77"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="77"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="80"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="80"/>
-      <c r="U7" s="84"/>
-      <c r="V7" s="84"/>
-      <c r="W7" s="84"/>
-      <c r="X7" s="84"/>
-      <c r="Y7" s="84"/>
-      <c r="Z7" s="84"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
+      <c r="N7" s="84"/>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="84"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="77"/>
+      <c r="W7" s="77"/>
+      <c r="X7" s="77"/>
+      <c r="Y7" s="77"/>
+      <c r="Z7" s="77"/>
     </row>
     <row r="8" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="63"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="89" t="s">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="91"/>
-      <c r="U8" s="84"/>
-      <c r="V8" s="84"/>
-      <c r="W8" s="84"/>
-      <c r="X8" s="84"/>
-      <c r="Y8" s="84"/>
-      <c r="Z8" s="84"/>
+      <c r="N8" s="86"/>
+      <c r="O8" s="86"/>
+      <c r="P8" s="86"/>
+      <c r="Q8" s="86"/>
+      <c r="R8" s="87"/>
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="77"/>
+      <c r="Z8" s="77"/>
     </row>
     <row r="9" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
@@ -6853,16 +6829,16 @@
       <c r="E9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="77" t="s">
+      <c r="G9" s="79"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
       <c r="L9" s="44" t="s">
         <v>124</v>
       </c>
@@ -6878,57 +6854,37 @@
       <c r="P9" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="Q9" s="85" t="s">
+      <c r="Q9" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="R9" s="87"/>
-      <c r="U9" s="84"/>
-      <c r="V9" s="84"/>
-      <c r="W9" s="84"/>
-      <c r="X9" s="84"/>
-      <c r="Y9" s="84"/>
-      <c r="Z9" s="84"/>
+      <c r="R9" s="80"/>
+      <c r="U9" s="77"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="77"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77"/>
+      <c r="Z9" s="77"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
-      <c r="B10" s="48" t="s">
-        <v>80</v>
-      </c>
+      <c r="B10" s="48"/>
       <c r="C10" s="48"/>
-      <c r="D10" s="48">
-        <v>2</v>
-      </c>
-      <c r="E10" s="48">
-        <v>4</v>
-      </c>
-      <c r="F10" s="48">
-        <v>0</v>
-      </c>
-      <c r="G10" s="48">
-        <v>0</v>
-      </c>
-      <c r="H10" s="48">
-        <v>0</v>
-      </c>
-      <c r="I10" s="48">
-        <v>663</v>
-      </c>
-      <c r="J10" s="48">
-        <v>0</v>
-      </c>
-      <c r="K10" s="48">
-        <v>0</v>
-      </c>
-      <c r="L10" s="48">
-        <v>0.5</v>
-      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
       <c r="M10" s="27"/>
-      <c r="U10" s="84"/>
-      <c r="V10" s="84"/>
-      <c r="W10" s="84"/>
-      <c r="X10" s="84"/>
-      <c r="Y10" s="84"/>
-      <c r="Z10" s="84"/>
+      <c r="U10" s="77"/>
+      <c r="V10" s="77"/>
+      <c r="W10" s="77"/>
+      <c r="X10" s="77"/>
+      <c r="Y10" s="77"/>
+      <c r="Z10" s="77"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
@@ -6943,49 +6899,49 @@
       <c r="J11" s="42"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
-      <c r="U11" s="84"/>
-      <c r="V11" s="84"/>
-      <c r="W11" s="84"/>
-      <c r="X11" s="84"/>
-      <c r="Y11" s="84"/>
-      <c r="Z11" s="84"/>
+      <c r="U11" s="77"/>
+      <c r="V11" s="77"/>
+      <c r="W11" s="77"/>
+      <c r="X11" s="77"/>
+      <c r="Y11" s="77"/>
+      <c r="Z11" s="77"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="U12" s="84"/>
-      <c r="V12" s="84"/>
-      <c r="W12" s="84"/>
-      <c r="X12" s="84"/>
-      <c r="Y12" s="84"/>
-      <c r="Z12" s="84"/>
+      <c r="U12" s="77"/>
+      <c r="V12" s="77"/>
+      <c r="W12" s="77"/>
+      <c r="X12" s="77"/>
+      <c r="Y12" s="77"/>
+      <c r="Z12" s="77"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="70"/>
-      <c r="M13" s="70"/>
-      <c r="N13" s="70"/>
-      <c r="O13" s="70"/>
-      <c r="P13" s="70"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="67"/>
       <c r="Q13" s="39"/>
       <c r="R13" s="39"/>
       <c r="S13" s="39"/>
-      <c r="U13" s="84"/>
-      <c r="V13" s="84"/>
-      <c r="W13" s="84"/>
-      <c r="X13" s="84"/>
-      <c r="Y13" s="84"/>
-      <c r="Z13" s="84"/>
+      <c r="U13" s="77"/>
+      <c r="V13" s="77"/>
+      <c r="W13" s="77"/>
+      <c r="X13" s="77"/>
+      <c r="Y13" s="77"/>
+      <c r="Z13" s="77"/>
     </row>
     <row r="14" spans="1:26" s="39" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
@@ -7003,24 +6959,24 @@
       <c r="E14" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
       <c r="I14" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="78" t="s">
+      <c r="J14" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-      <c r="M14" s="78" t="s">
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="N14" s="78"/>
-      <c r="O14" s="78"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
       <c r="P14" s="40" t="s">
         <v>86</v>
       </c>
@@ -7069,6 +7025,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="M2:R2"/>
     <mergeCell ref="U2:Z13"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="I3:K3"/>
@@ -7080,12 +7042,6 @@
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="A13:P13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="M2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>